<commit_message>
aggiunta gestione immagine su db, popolamento di immagini, insert e select con creazione di file locale
</commit_message>
<xml_diff>
--- a/SoftwareSanitario/database/excel/patient_data.xlsx
+++ b/SoftwareSanitario/database/excel/patient_data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="88" documentId="11_AD4D5CB4E552A52AC6156845DA9857005BDEDDA4" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{43A6C9CF-CD0E-439B-BD89-17ADD095EED7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{63B1451C-C3C2-473C-AE18-A2E505F90BE3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4956" yWindow="2580" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -970,7 +970,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -982,7 +982,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1263,10 +1262,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J100"/>
+  <dimension ref="A1:I100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F100"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1275,11 +1274,11 @@
     <col min="3" max="3" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5546875" customWidth="1"/>
     <col min="6" max="6" width="8.88671875" customWidth="1"/>
-    <col min="9" max="9" width="22.21875" style="5" customWidth="1"/>
-    <col min="10" max="10" width="23.33203125" customWidth="1"/>
+    <col min="8" max="8" width="22.21875" style="5" customWidth="1"/>
+    <col min="9" max="9" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1302,17 +1301,14 @@
       <c r="G1" t="s">
         <v>197</v>
       </c>
-      <c r="H1" s="7">
-        <v>1</v>
-      </c>
-      <c r="I1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="J1" t="s">
+      <c r="I1" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1336,17 +1332,14 @@
       <c r="G2" t="s">
         <v>197</v>
       </c>
-      <c r="H2" s="7">
-        <v>1</v>
-      </c>
-      <c r="I2" s="6" t="s">
+      <c r="H2" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="J2" t="s">
+      <c r="I2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1370,17 +1363,14 @@
       <c r="G3" t="s">
         <v>197</v>
       </c>
-      <c r="H3" s="7">
-        <v>1</v>
-      </c>
-      <c r="I3" s="6" t="s">
+      <c r="H3" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="J3" t="s">
+      <c r="I3" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1404,17 +1394,14 @@
       <c r="G4" t="s">
         <v>197</v>
       </c>
-      <c r="H4" s="7">
-        <v>1</v>
-      </c>
-      <c r="I4" s="6" t="s">
+      <c r="H4" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="J4" t="s">
+      <c r="I4" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1438,17 +1425,14 @@
       <c r="G5" t="s">
         <v>197</v>
       </c>
-      <c r="H5" s="7">
-        <v>1</v>
-      </c>
-      <c r="I5" s="6" t="s">
+      <c r="H5" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="J5" t="s">
+      <c r="I5" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1472,17 +1456,14 @@
       <c r="G6" t="s">
         <v>197</v>
       </c>
-      <c r="H6" s="7">
-        <v>1</v>
-      </c>
-      <c r="I6" s="6" t="s">
+      <c r="H6" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="J6" t="s">
+      <c r="I6" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1506,17 +1487,14 @@
       <c r="G7" t="s">
         <v>197</v>
       </c>
-      <c r="H7" s="7">
-        <v>1</v>
-      </c>
-      <c r="I7" s="6" t="s">
+      <c r="H7" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="J7" t="s">
+      <c r="I7" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1540,17 +1518,14 @@
       <c r="G8" t="s">
         <v>197</v>
       </c>
-      <c r="H8" s="7">
-        <v>1</v>
-      </c>
-      <c r="I8" s="6" t="s">
+      <c r="H8" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="J8" t="s">
+      <c r="I8" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1574,17 +1549,14 @@
       <c r="G9" t="s">
         <v>197</v>
       </c>
-      <c r="H9" s="7">
-        <v>1</v>
-      </c>
-      <c r="I9" s="6" t="s">
+      <c r="H9" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="J9" t="s">
+      <c r="I9" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1608,17 +1580,14 @@
       <c r="G10" t="s">
         <v>197</v>
       </c>
-      <c r="H10" s="7">
-        <v>1</v>
-      </c>
-      <c r="I10" s="6" t="s">
+      <c r="H10" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="J10" t="s">
+      <c r="I10" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1642,17 +1611,14 @@
       <c r="G11" t="s">
         <v>197</v>
       </c>
-      <c r="H11" s="7">
-        <v>1</v>
-      </c>
-      <c r="I11" s="6" t="s">
+      <c r="H11" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="J11" t="s">
+      <c r="I11" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1676,17 +1642,14 @@
       <c r="G12" t="s">
         <v>197</v>
       </c>
-      <c r="H12" s="7">
-        <v>1</v>
-      </c>
-      <c r="I12" s="6" t="s">
+      <c r="H12" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="J12" t="s">
+      <c r="I12" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1710,17 +1673,14 @@
       <c r="G13" t="s">
         <v>197</v>
       </c>
-      <c r="H13" s="7">
-        <v>1</v>
-      </c>
-      <c r="I13" s="6" t="s">
+      <c r="H13" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="J13" t="s">
+      <c r="I13" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1744,17 +1704,14 @@
       <c r="G14" t="s">
         <v>197</v>
       </c>
-      <c r="H14" s="7">
-        <v>1</v>
-      </c>
-      <c r="I14" s="6" t="s">
+      <c r="H14" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="J14" t="s">
+      <c r="I14" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1778,17 +1735,14 @@
       <c r="G15" t="s">
         <v>197</v>
       </c>
-      <c r="H15" s="7">
-        <v>1</v>
-      </c>
-      <c r="I15" s="6" t="s">
+      <c r="H15" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="J15" t="s">
+      <c r="I15" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -1812,17 +1766,14 @@
       <c r="G16" t="s">
         <v>197</v>
       </c>
-      <c r="H16" s="7">
-        <v>1</v>
-      </c>
-      <c r="I16" s="6" t="s">
+      <c r="H16" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="J16" t="s">
+      <c r="I16" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1846,17 +1797,14 @@
       <c r="G17" t="s">
         <v>197</v>
       </c>
-      <c r="H17" s="7">
-        <v>1</v>
-      </c>
-      <c r="I17" s="6" t="s">
+      <c r="H17" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="J17" t="s">
+      <c r="I17" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1880,17 +1828,14 @@
       <c r="G18" t="s">
         <v>197</v>
       </c>
-      <c r="H18" s="7">
-        <v>1</v>
-      </c>
-      <c r="I18" s="6" t="s">
+      <c r="H18" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="J18" t="s">
+      <c r="I18" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -1914,17 +1859,14 @@
       <c r="G19" t="s">
         <v>197</v>
       </c>
-      <c r="H19" s="7">
-        <v>1</v>
-      </c>
-      <c r="I19" s="6" t="s">
+      <c r="H19" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="J19" t="s">
+      <c r="I19" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
@@ -1948,17 +1890,14 @@
       <c r="G20" t="s">
         <v>197</v>
       </c>
-      <c r="H20" s="7">
-        <v>1</v>
-      </c>
-      <c r="I20" s="6" t="s">
+      <c r="H20" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="J20" t="s">
+      <c r="I20" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -1982,17 +1921,14 @@
       <c r="G21" t="s">
         <v>197</v>
       </c>
-      <c r="H21" s="7">
-        <v>1</v>
-      </c>
-      <c r="I21" s="6" t="s">
+      <c r="H21" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="J21" t="s">
+      <c r="I21" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -2016,17 +1952,14 @@
       <c r="G22" t="s">
         <v>197</v>
       </c>
-      <c r="H22" s="7">
-        <v>1</v>
-      </c>
-      <c r="I22" s="6" t="s">
+      <c r="H22" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="J22" t="s">
+      <c r="I22" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -2050,17 +1983,14 @@
       <c r="G23" t="s">
         <v>197</v>
       </c>
-      <c r="H23" s="7">
-        <v>1</v>
-      </c>
-      <c r="I23" s="6" t="s">
+      <c r="H23" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="J23" t="s">
+      <c r="I23" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -2084,17 +2014,14 @@
       <c r="G24" t="s">
         <v>197</v>
       </c>
-      <c r="H24" s="7">
-        <v>1</v>
-      </c>
-      <c r="I24" s="6" t="s">
+      <c r="H24" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="J24" t="s">
+      <c r="I24" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -2118,17 +2045,14 @@
       <c r="G25" t="s">
         <v>197</v>
       </c>
-      <c r="H25" s="7">
-        <v>1</v>
-      </c>
-      <c r="I25" s="6" t="s">
+      <c r="H25" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="J25" t="s">
+      <c r="I25" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -2152,17 +2076,14 @@
       <c r="G26" t="s">
         <v>197</v>
       </c>
-      <c r="H26" s="7">
-        <v>1</v>
-      </c>
-      <c r="I26" s="6" t="s">
+      <c r="H26" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="J26" t="s">
+      <c r="I26" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -2186,17 +2107,14 @@
       <c r="G27" t="s">
         <v>197</v>
       </c>
-      <c r="H27" s="7">
-        <v>1</v>
-      </c>
-      <c r="I27" s="6" t="s">
+      <c r="H27" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="J27" t="s">
+      <c r="I27" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
@@ -2220,17 +2138,14 @@
       <c r="G28" t="s">
         <v>197</v>
       </c>
-      <c r="H28" s="7">
-        <v>1</v>
-      </c>
-      <c r="I28" s="6" t="s">
+      <c r="H28" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="J28" t="s">
+      <c r="I28" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -2254,17 +2169,14 @@
       <c r="G29" t="s">
         <v>197</v>
       </c>
-      <c r="H29" s="7">
-        <v>1</v>
-      </c>
-      <c r="I29" s="6" t="s">
+      <c r="H29" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="J29" t="s">
+      <c r="I29" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
@@ -2288,17 +2200,14 @@
       <c r="G30" t="s">
         <v>197</v>
       </c>
-      <c r="H30" s="7">
-        <v>1</v>
-      </c>
-      <c r="I30" s="6" t="s">
+      <c r="H30" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="J30" t="s">
+      <c r="I30" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
@@ -2322,17 +2231,14 @@
       <c r="G31" t="s">
         <v>197</v>
       </c>
-      <c r="H31" s="7">
-        <v>1</v>
-      </c>
-      <c r="I31" s="6" t="s">
+      <c r="H31" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="J31" t="s">
+      <c r="I31" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -2356,17 +2262,14 @@
       <c r="G32" t="s">
         <v>197</v>
       </c>
-      <c r="H32" s="7">
-        <v>1</v>
-      </c>
-      <c r="I32" s="6" t="s">
+      <c r="H32" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="J32" t="s">
+      <c r="I32" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
@@ -2390,17 +2293,14 @@
       <c r="G33" t="s">
         <v>197</v>
       </c>
-      <c r="H33" s="7">
-        <v>1</v>
-      </c>
-      <c r="I33" s="6" t="s">
+      <c r="H33" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="J33" t="s">
+      <c r="I33" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
@@ -2424,17 +2324,14 @@
       <c r="G34" t="s">
         <v>197</v>
       </c>
-      <c r="H34" s="7">
-        <v>1</v>
-      </c>
-      <c r="I34" s="6" t="s">
+      <c r="H34" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="J34" t="s">
+      <c r="I34" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
@@ -2458,17 +2355,14 @@
       <c r="G35" t="s">
         <v>197</v>
       </c>
-      <c r="H35" s="7">
-        <v>1</v>
-      </c>
-      <c r="I35" s="6" t="s">
+      <c r="H35" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="J35" t="s">
+      <c r="I35" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
@@ -2492,17 +2386,14 @@
       <c r="G36" t="s">
         <v>197</v>
       </c>
-      <c r="H36" s="7">
-        <v>1</v>
-      </c>
-      <c r="I36" s="6" t="s">
+      <c r="H36" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="J36" t="s">
+      <c r="I36" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
@@ -2526,17 +2417,14 @@
       <c r="G37" t="s">
         <v>197</v>
       </c>
-      <c r="H37" s="7">
-        <v>1</v>
-      </c>
-      <c r="I37" s="6" t="s">
+      <c r="H37" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="J37" t="s">
+      <c r="I37" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
@@ -2560,17 +2448,14 @@
       <c r="G38" t="s">
         <v>197</v>
       </c>
-      <c r="H38" s="7">
-        <v>1</v>
-      </c>
-      <c r="I38" s="6" t="s">
+      <c r="H38" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="J38" t="s">
+      <c r="I38" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
@@ -2594,17 +2479,14 @@
       <c r="G39" t="s">
         <v>197</v>
       </c>
-      <c r="H39" s="7">
-        <v>1</v>
-      </c>
-      <c r="I39" s="6" t="s">
+      <c r="H39" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="J39" t="s">
+      <c r="I39" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
@@ -2628,17 +2510,14 @@
       <c r="G40" t="s">
         <v>197</v>
       </c>
-      <c r="H40" s="7">
-        <v>1</v>
-      </c>
-      <c r="I40" s="6" t="s">
+      <c r="H40" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="J40" t="s">
+      <c r="I40" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>40</v>
       </c>
@@ -2662,17 +2541,14 @@
       <c r="G41" t="s">
         <v>197</v>
       </c>
-      <c r="H41" s="7">
-        <v>1</v>
-      </c>
-      <c r="I41" s="6" t="s">
+      <c r="H41" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="J41" t="s">
+      <c r="I41" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>41</v>
       </c>
@@ -2696,17 +2572,14 @@
       <c r="G42" t="s">
         <v>197</v>
       </c>
-      <c r="H42" s="7">
-        <v>1</v>
-      </c>
-      <c r="I42" s="6" t="s">
+      <c r="H42" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="J42" t="s">
+      <c r="I42" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
@@ -2730,17 +2603,14 @@
       <c r="G43" t="s">
         <v>197</v>
       </c>
-      <c r="H43" s="7">
-        <v>1</v>
-      </c>
-      <c r="I43" s="6" t="s">
+      <c r="H43" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="J43" t="s">
+      <c r="I43" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>43</v>
       </c>
@@ -2764,17 +2634,14 @@
       <c r="G44" t="s">
         <v>197</v>
       </c>
-      <c r="H44" s="7">
-        <v>1</v>
-      </c>
-      <c r="I44" s="6" t="s">
+      <c r="H44" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="J44" t="s">
+      <c r="I44" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>44</v>
       </c>
@@ -2798,17 +2665,14 @@
       <c r="G45" t="s">
         <v>197</v>
       </c>
-      <c r="H45" s="7">
-        <v>1</v>
-      </c>
-      <c r="I45" s="6" t="s">
+      <c r="H45" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="J45" t="s">
+      <c r="I45" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
@@ -2832,17 +2696,14 @@
       <c r="G46" t="s">
         <v>197</v>
       </c>
-      <c r="H46" s="7">
-        <v>1</v>
-      </c>
-      <c r="I46" s="6" t="s">
+      <c r="H46" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="J46" t="s">
+      <c r="I46" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
@@ -2866,17 +2727,14 @@
       <c r="G47" t="s">
         <v>197</v>
       </c>
-      <c r="H47" s="7">
-        <v>1</v>
-      </c>
-      <c r="I47" s="6" t="s">
+      <c r="H47" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="J47" t="s">
+      <c r="I47" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>47</v>
       </c>
@@ -2900,17 +2758,14 @@
       <c r="G48" t="s">
         <v>197</v>
       </c>
-      <c r="H48" s="7">
-        <v>1</v>
-      </c>
-      <c r="I48" s="6" t="s">
+      <c r="H48" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="J48" t="s">
+      <c r="I48" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>48</v>
       </c>
@@ -2934,17 +2789,14 @@
       <c r="G49" t="s">
         <v>197</v>
       </c>
-      <c r="H49" s="7">
-        <v>1</v>
-      </c>
-      <c r="I49" s="6" t="s">
+      <c r="H49" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="J49" t="s">
+      <c r="I49" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
@@ -2968,17 +2820,14 @@
       <c r="G50" t="s">
         <v>197</v>
       </c>
-      <c r="H50" s="7">
-        <v>1</v>
-      </c>
-      <c r="I50" s="6" t="s">
+      <c r="H50" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="J50" t="s">
+      <c r="I50" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
@@ -3002,17 +2851,14 @@
       <c r="G51" t="s">
         <v>197</v>
       </c>
-      <c r="H51" s="7">
-        <v>1</v>
-      </c>
-      <c r="I51" s="6" t="s">
+      <c r="H51" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="J51" t="s">
+      <c r="I51" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>51</v>
       </c>
@@ -3036,17 +2882,14 @@
       <c r="G52" t="s">
         <v>197</v>
       </c>
-      <c r="H52" s="7">
-        <v>1</v>
-      </c>
-      <c r="I52" s="6" t="s">
+      <c r="H52" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="J52" t="s">
+      <c r="I52" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>52</v>
       </c>
@@ -3070,17 +2913,14 @@
       <c r="G53" t="s">
         <v>197</v>
       </c>
-      <c r="H53" s="7">
-        <v>1</v>
-      </c>
-      <c r="I53" s="6" t="s">
+      <c r="H53" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="J53" t="s">
+      <c r="I53" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>53</v>
       </c>
@@ -3104,17 +2944,14 @@
       <c r="G54" t="s">
         <v>197</v>
       </c>
-      <c r="H54" s="7">
-        <v>1</v>
-      </c>
-      <c r="I54" s="6" t="s">
+      <c r="H54" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="J54" t="s">
+      <c r="I54" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>54</v>
       </c>
@@ -3138,17 +2975,14 @@
       <c r="G55" t="s">
         <v>197</v>
       </c>
-      <c r="H55" s="7">
-        <v>1</v>
-      </c>
-      <c r="I55" s="6" t="s">
+      <c r="H55" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="J55" t="s">
+      <c r="I55" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>55</v>
       </c>
@@ -3172,17 +3006,14 @@
       <c r="G56" t="s">
         <v>197</v>
       </c>
-      <c r="H56" s="7">
-        <v>1</v>
-      </c>
-      <c r="I56" s="6" t="s">
+      <c r="H56" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="J56" t="s">
+      <c r="I56" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>56</v>
       </c>
@@ -3206,17 +3037,14 @@
       <c r="G57" t="s">
         <v>197</v>
       </c>
-      <c r="H57" s="7">
-        <v>1</v>
-      </c>
-      <c r="I57" s="6" t="s">
+      <c r="H57" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="J57" t="s">
+      <c r="I57" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>57</v>
       </c>
@@ -3240,17 +3068,14 @@
       <c r="G58" t="s">
         <v>197</v>
       </c>
-      <c r="H58" s="7">
-        <v>1</v>
-      </c>
-      <c r="I58" s="6" t="s">
+      <c r="H58" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="J58" t="s">
+      <c r="I58" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>58</v>
       </c>
@@ -3274,17 +3099,14 @@
       <c r="G59" t="s">
         <v>197</v>
       </c>
-      <c r="H59" s="7">
-        <v>1</v>
-      </c>
-      <c r="I59" s="6" t="s">
+      <c r="H59" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="J59" t="s">
+      <c r="I59" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>59</v>
       </c>
@@ -3308,17 +3130,14 @@
       <c r="G60" t="s">
         <v>197</v>
       </c>
-      <c r="H60" s="7">
-        <v>1</v>
-      </c>
-      <c r="I60" s="6" t="s">
+      <c r="H60" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="J60" t="s">
+      <c r="I60" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>60</v>
       </c>
@@ -3342,17 +3161,14 @@
       <c r="G61" t="s">
         <v>197</v>
       </c>
-      <c r="H61" s="7">
-        <v>1</v>
-      </c>
-      <c r="I61" s="6" t="s">
+      <c r="H61" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="J61" t="s">
+      <c r="I61" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>61</v>
       </c>
@@ -3376,17 +3192,14 @@
       <c r="G62" t="s">
         <v>197</v>
       </c>
-      <c r="H62" s="7">
-        <v>1</v>
-      </c>
-      <c r="I62" s="6" t="s">
+      <c r="H62" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="J62" t="s">
+      <c r="I62" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>62</v>
       </c>
@@ -3410,17 +3223,14 @@
       <c r="G63" t="s">
         <v>197</v>
       </c>
-      <c r="H63" s="7">
-        <v>1</v>
-      </c>
-      <c r="I63" s="6" t="s">
+      <c r="H63" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="J63" t="s">
+      <c r="I63" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>63</v>
       </c>
@@ -3444,17 +3254,14 @@
       <c r="G64" t="s">
         <v>197</v>
       </c>
-      <c r="H64" s="7">
-        <v>1</v>
-      </c>
-      <c r="I64" s="6" t="s">
+      <c r="H64" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="J64" t="s">
+      <c r="I64" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>64</v>
       </c>
@@ -3478,17 +3285,14 @@
       <c r="G65" t="s">
         <v>197</v>
       </c>
-      <c r="H65" s="7">
-        <v>1</v>
-      </c>
-      <c r="I65" s="6" t="s">
+      <c r="H65" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="J65" t="s">
+      <c r="I65" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>65</v>
       </c>
@@ -3512,17 +3316,14 @@
       <c r="G66" t="s">
         <v>197</v>
       </c>
-      <c r="H66" s="7">
-        <v>1</v>
-      </c>
-      <c r="I66" s="6" t="s">
+      <c r="H66" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="J66" t="s">
+      <c r="I66" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>66</v>
       </c>
@@ -3546,17 +3347,14 @@
       <c r="G67" t="s">
         <v>197</v>
       </c>
-      <c r="H67" s="7">
-        <v>1</v>
-      </c>
-      <c r="I67" s="6" t="s">
+      <c r="H67" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="J67" t="s">
+      <c r="I67" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>67</v>
       </c>
@@ -3580,17 +3378,14 @@
       <c r="G68" t="s">
         <v>197</v>
       </c>
-      <c r="H68" s="7">
-        <v>1</v>
-      </c>
-      <c r="I68" s="6" t="s">
+      <c r="H68" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="J68" t="s">
+      <c r="I68" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>68</v>
       </c>
@@ -3614,17 +3409,14 @@
       <c r="G69" t="s">
         <v>197</v>
       </c>
-      <c r="H69" s="7">
-        <v>1</v>
-      </c>
-      <c r="I69" s="6" t="s">
+      <c r="H69" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="J69" t="s">
+      <c r="I69" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>69</v>
       </c>
@@ -3648,17 +3440,14 @@
       <c r="G70" t="s">
         <v>197</v>
       </c>
-      <c r="H70" s="7">
-        <v>1</v>
-      </c>
-      <c r="I70" s="6" t="s">
+      <c r="H70" s="6" t="s">
         <v>299</v>
       </c>
-      <c r="J70" t="s">
+      <c r="I70" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>70</v>
       </c>
@@ -3682,17 +3471,14 @@
       <c r="G71" t="s">
         <v>197</v>
       </c>
-      <c r="H71" s="7">
-        <v>1</v>
-      </c>
-      <c r="I71" s="6" t="s">
+      <c r="H71" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="J71" t="s">
+      <c r="I71" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>71</v>
       </c>
@@ -3716,17 +3502,14 @@
       <c r="G72" t="s">
         <v>197</v>
       </c>
-      <c r="H72" s="7">
-        <v>1</v>
-      </c>
-      <c r="I72" s="6" t="s">
+      <c r="H72" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="J72" t="s">
+      <c r="I72" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>72</v>
       </c>
@@ -3750,17 +3533,14 @@
       <c r="G73" t="s">
         <v>197</v>
       </c>
-      <c r="H73" s="7">
-        <v>1</v>
-      </c>
-      <c r="I73" s="6" t="s">
+      <c r="H73" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="J73" t="s">
+      <c r="I73" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>58</v>
       </c>
@@ -3784,17 +3564,14 @@
       <c r="G74" t="s">
         <v>197</v>
       </c>
-      <c r="H74" s="7">
-        <v>1</v>
-      </c>
-      <c r="I74" s="6" t="s">
+      <c r="H74" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="J74" t="s">
+      <c r="I74" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>73</v>
       </c>
@@ -3818,17 +3595,14 @@
       <c r="G75" t="s">
         <v>197</v>
       </c>
-      <c r="H75" s="7">
-        <v>1</v>
-      </c>
-      <c r="I75" s="6" t="s">
+      <c r="H75" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="J75" t="s">
+      <c r="I75" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>74</v>
       </c>
@@ -3852,17 +3626,14 @@
       <c r="G76" t="s">
         <v>197</v>
       </c>
-      <c r="H76" s="7">
-        <v>1</v>
-      </c>
-      <c r="I76" s="6" t="s">
+      <c r="H76" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="J76" t="s">
+      <c r="I76" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>75</v>
       </c>
@@ -3886,17 +3657,14 @@
       <c r="G77" t="s">
         <v>197</v>
       </c>
-      <c r="H77" s="7">
-        <v>1</v>
-      </c>
-      <c r="I77" s="6" t="s">
+      <c r="H77" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="J77" t="s">
+      <c r="I77" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>76</v>
       </c>
@@ -3920,17 +3688,14 @@
       <c r="G78" t="s">
         <v>197</v>
       </c>
-      <c r="H78" s="7">
-        <v>1</v>
-      </c>
-      <c r="I78" s="6" t="s">
+      <c r="H78" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="J78" t="s">
+      <c r="I78" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>77</v>
       </c>
@@ -3954,17 +3719,14 @@
       <c r="G79" t="s">
         <v>197</v>
       </c>
-      <c r="H79" s="7">
-        <v>1</v>
-      </c>
-      <c r="I79" s="6" t="s">
+      <c r="H79" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="J79" t="s">
+      <c r="I79" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>78</v>
       </c>
@@ -3988,17 +3750,14 @@
       <c r="G80" t="s">
         <v>197</v>
       </c>
-      <c r="H80" s="7">
-        <v>1</v>
-      </c>
-      <c r="I80" s="6" t="s">
+      <c r="H80" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="J80" t="s">
+      <c r="I80" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>79</v>
       </c>
@@ -4022,17 +3781,14 @@
       <c r="G81" t="s">
         <v>197</v>
       </c>
-      <c r="H81" s="7">
-        <v>1</v>
-      </c>
-      <c r="I81" s="6" t="s">
+      <c r="H81" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="J81" t="s">
+      <c r="I81" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>80</v>
       </c>
@@ -4056,17 +3812,14 @@
       <c r="G82" t="s">
         <v>197</v>
       </c>
-      <c r="H82" s="7">
-        <v>1</v>
-      </c>
-      <c r="I82" s="6" t="s">
+      <c r="H82" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="J82" t="s">
+      <c r="I82" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>81</v>
       </c>
@@ -4090,17 +3843,14 @@
       <c r="G83" t="s">
         <v>197</v>
       </c>
-      <c r="H83" s="7">
-        <v>1</v>
-      </c>
-      <c r="I83" s="6" t="s">
+      <c r="H83" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="J83" t="s">
+      <c r="I83" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>82</v>
       </c>
@@ -4124,17 +3874,14 @@
       <c r="G84" t="s">
         <v>197</v>
       </c>
-      <c r="H84" s="7">
-        <v>1</v>
-      </c>
-      <c r="I84" s="6" t="s">
+      <c r="H84" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="J84" t="s">
+      <c r="I84" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>83</v>
       </c>
@@ -4158,17 +3905,14 @@
       <c r="G85" t="s">
         <v>197</v>
       </c>
-      <c r="H85" s="7">
-        <v>1</v>
-      </c>
-      <c r="I85" s="6" t="s">
+      <c r="H85" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="J85" t="s">
+      <c r="I85" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>84</v>
       </c>
@@ -4192,17 +3936,14 @@
       <c r="G86" t="s">
         <v>197</v>
       </c>
-      <c r="H86" s="7">
-        <v>1</v>
-      </c>
-      <c r="I86" s="6" t="s">
+      <c r="H86" s="6" t="s">
         <v>300</v>
       </c>
-      <c r="J86" t="s">
+      <c r="I86" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>85</v>
       </c>
@@ -4226,17 +3967,14 @@
       <c r="G87" t="s">
         <v>197</v>
       </c>
-      <c r="H87" s="7">
-        <v>1</v>
-      </c>
-      <c r="I87" s="6" t="s">
+      <c r="H87" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="J87" t="s">
+      <c r="I87" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>86</v>
       </c>
@@ -4260,17 +3998,14 @@
       <c r="G88" t="s">
         <v>197</v>
       </c>
-      <c r="H88" s="7">
-        <v>1</v>
-      </c>
-      <c r="I88" s="6" t="s">
+      <c r="H88" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="J88" t="s">
+      <c r="I88" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>87</v>
       </c>
@@ -4294,17 +4029,14 @@
       <c r="G89" t="s">
         <v>197</v>
       </c>
-      <c r="H89" s="7">
-        <v>1</v>
-      </c>
-      <c r="I89" s="6" t="s">
+      <c r="H89" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="J89" t="s">
+      <c r="I89" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>88</v>
       </c>
@@ -4328,17 +4060,14 @@
       <c r="G90" t="s">
         <v>197</v>
       </c>
-      <c r="H90" s="7">
-        <v>1</v>
-      </c>
-      <c r="I90" s="6" t="s">
+      <c r="H90" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="J90" t="s">
+      <c r="I90" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>89</v>
       </c>
@@ -4362,17 +4091,14 @@
       <c r="G91" t="s">
         <v>197</v>
       </c>
-      <c r="H91" s="7">
-        <v>1</v>
-      </c>
-      <c r="I91" s="6" t="s">
+      <c r="H91" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="J91" t="s">
+      <c r="I91" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>90</v>
       </c>
@@ -4396,17 +4122,14 @@
       <c r="G92" t="s">
         <v>197</v>
       </c>
-      <c r="H92" s="7">
-        <v>1</v>
-      </c>
-      <c r="I92" s="6" t="s">
+      <c r="H92" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="J92" t="s">
+      <c r="I92" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>91</v>
       </c>
@@ -4430,17 +4153,14 @@
       <c r="G93" t="s">
         <v>197</v>
       </c>
-      <c r="H93" s="7">
-        <v>1</v>
-      </c>
-      <c r="I93" s="6" t="s">
+      <c r="H93" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="J93" t="s">
+      <c r="I93" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>92</v>
       </c>
@@ -4464,17 +4184,14 @@
       <c r="G94" t="s">
         <v>197</v>
       </c>
-      <c r="H94" s="7">
-        <v>1</v>
-      </c>
-      <c r="I94" s="6" t="s">
+      <c r="H94" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="J94" t="s">
+      <c r="I94" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>93</v>
       </c>
@@ -4498,17 +4215,14 @@
       <c r="G95" t="s">
         <v>197</v>
       </c>
-      <c r="H95" s="7">
-        <v>1</v>
-      </c>
-      <c r="I95" s="6" t="s">
+      <c r="H95" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="J95" t="s">
+      <c r="I95" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>94</v>
       </c>
@@ -4532,17 +4246,14 @@
       <c r="G96" t="s">
         <v>197</v>
       </c>
-      <c r="H96" s="7">
-        <v>1</v>
-      </c>
-      <c r="I96" s="6" t="s">
+      <c r="H96" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="J96" t="s">
+      <c r="I96" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>95</v>
       </c>
@@ -4566,17 +4277,14 @@
       <c r="G97" t="s">
         <v>197</v>
       </c>
-      <c r="H97" s="7">
-        <v>1</v>
-      </c>
-      <c r="I97" s="6" t="s">
+      <c r="H97" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="J97" t="s">
+      <c r="I97" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>96</v>
       </c>
@@ -4600,17 +4308,14 @@
       <c r="G98" t="s">
         <v>197</v>
       </c>
-      <c r="H98" s="7">
-        <v>1</v>
-      </c>
-      <c r="I98" s="6" t="s">
+      <c r="H98" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="J98" t="s">
+      <c r="I98" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>97</v>
       </c>
@@ -4634,17 +4339,14 @@
       <c r="G99" t="s">
         <v>197</v>
       </c>
-      <c r="H99" s="7">
-        <v>1</v>
-      </c>
-      <c r="I99" s="6" t="s">
+      <c r="H99" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="J99" t="s">
+      <c r="I99" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>98</v>
       </c>
@@ -4668,13 +4370,10 @@
       <c r="G100" t="s">
         <v>197</v>
       </c>
-      <c r="H100" s="7">
-        <v>1</v>
-      </c>
-      <c r="I100" s="6" t="s">
+      <c r="H100" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="J100" t="s">
+      <c r="I100" t="s">
         <v>295</v>
       </c>
     </row>
@@ -4682,4 +4381,272 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101008F1D26AA9063C44D9D7B42AEE879C6CD" ma:contentTypeVersion="11" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="2f80071aa66f82567bdcc22d9883f7f5">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="e25ae402-d948-4387-b4ab-867d700f3c2b" xmlns:ns4="e30140dd-c666-4ff3-ac60-2216e57fdebb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1e666f408171dadceff32507896a4d13" ns3:_="" ns4:_="">
+    <xsd:import namespace="e25ae402-d948-4387-b4ab-867d700f3c2b"/>
+    <xsd:import namespace="e30140dd-c666-4ff3-ac60-2216e57fdebb"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns4:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns4:SharingHintHash" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="e25ae402-d948-4387-b4ab-867d700f3c2b" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:description="" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:description="" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:description="" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="11" nillable="true" ma:displayName="MediaServiceAutoTags" ma:description="" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="12" nillable="true" ma:displayName="MediaServiceOCR" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="13" nillable="true" ma:displayName="MediaServiceLocation" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="e30140dd-c666-4ff3-ac60-2216e57fdebb" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="14" nillable="true" ma:displayName="Condiviso con" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="15" nillable="true" ma:displayName="Condiviso con dettagli" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SharingHintHash" ma:index="16" nillable="true" ma:displayName="Hash suggerimento condivisione" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo di contenuto"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titolo"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{344C7296-4309-4A2C-B7B2-EA5CE300B928}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e25ae402-d948-4387-b4ab-867d700f3c2b"/>
+    <ds:schemaRef ds:uri="e30140dd-c666-4ff3-ac60-2216e57fdebb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6F97287-0137-4FBF-90B9-063A710031A8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{72E3D5A5-1F36-450E-A065-99A0D15D20E1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="e30140dd-c666-4ff3-ac60-2216e57fdebb"/>
+    <ds:schemaRef ds:uri="e25ae402-d948-4387-b4ab-867d700f3c2b"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>